<commit_message>
Criado interfae gráfica com customtkinter
</commit_message>
<xml_diff>
--- a/output/logs.xlsx
+++ b/output/logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1689,13 +1689,190 @@
           <t>Invoice1.pdf</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
           <t>Exception</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
+        <is>
+          <t>Invoice outside the specified standard: 'NoneType' object has no attribute 'group'</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>18:48:12</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>invoice.pdf</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:48:13</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Invoice1.pdf</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Exception</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Invoice outside the specified standard: 'NoneType' object has no attribute 'group'</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>18:49:16</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>invoice.pdf</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>18:49:16</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Invoice1.pdf</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Exception</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Invoice outside the specified standard: 'NoneType' object has no attribute 'group'</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>19:31:24</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>invoice.pdf</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>19:31:25</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Invoice1.pdf</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Exception</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t>Invoice outside the specified standard: 'NoneType' object has no attribute 'group'</t>
         </is>

</xml_diff>